<commit_message>
corrected cap2act for transport
</commit_message>
<xml_diff>
--- a/config_data/mapping_v3.xlsx
+++ b/config_data/mapping_v3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8148"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="SEDOS_parameters" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">commodity_set!$A$1:$A$130</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="309">
   <si>
     <t>TIMES</t>
   </si>
@@ -558,9 +558,6 @@
     <t>S_EFF</t>
   </si>
   <si>
-    <t>occupancy</t>
-  </si>
-  <si>
     <t>UC</t>
   </si>
   <si>
@@ -1015,6 +1012,12 @@
   </si>
   <si>
     <t>exo_agri_livestock</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>ACTFLO~DEMO</t>
   </si>
 </sst>
 </file>
@@ -1517,24 +1520,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1566,18 +1569,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>81</v>
       </c>
@@ -1599,10 +1602,10 @@
         <v>82</v>
       </c>
       <c r="J4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>101</v>
       </c>
@@ -1610,7 +1613,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I5" t="s">
         <v>19</v>
@@ -1620,23 +1623,23 @@
       </c>
       <c r="N5" s="9"/>
       <c r="O5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N6" s="7"/>
       <c r="O6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1647,16 +1650,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>74</v>
       </c>
@@ -1664,10 +1667,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>103</v>
       </c>
@@ -1675,13 +1678,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>104</v>
       </c>
@@ -1689,13 +1692,13 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
@@ -1706,7 +1709,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>105</v>
       </c>
@@ -1714,13 +1717,13 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>106</v>
       </c>
@@ -1728,13 +1731,13 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>56</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>107</v>
       </c>
@@ -1753,13 +1756,13 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>108</v>
       </c>
@@ -1767,13 +1770,13 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>109</v>
       </c>
@@ -1781,10 +1784,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
@@ -1792,13 +1795,13 @@
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -1812,7 +1815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -1826,7 +1829,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1837,7 +1840,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>110</v>
       </c>
@@ -1845,10 +1848,10 @@
         <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>111</v>
       </c>
@@ -1856,22 +1859,22 @@
         <v>150</v>
       </c>
       <c r="C24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J25" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -1882,7 +1885,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>66</v>
       </c>
@@ -1893,7 +1896,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>59</v>
       </c>
@@ -1904,7 +1907,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>113</v>
       </c>
@@ -1912,10 +1915,10 @@
         <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>78</v>
       </c>
@@ -1926,7 +1929,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>68</v>
       </c>
@@ -1937,7 +1940,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
@@ -1948,7 +1951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>114</v>
       </c>
@@ -1956,10 +1959,10 @@
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>70</v>
       </c>
@@ -1970,7 +1973,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>115</v>
       </c>
@@ -1978,7 +1981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>61</v>
       </c>
@@ -1989,7 +1992,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>116</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>117</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>118</v>
       </c>
@@ -2028,7 +2031,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>119</v>
       </c>
@@ -2042,7 +2045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -2050,10 +2053,10 @@
         <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>121</v>
       </c>
@@ -2061,24 +2064,24 @@
         <v>151</v>
       </c>
       <c r="C42" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>123</v>
       </c>
@@ -2086,10 +2089,10 @@
         <v>153</v>
       </c>
       <c r="C44" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>124</v>
       </c>
@@ -2097,373 +2100,373 @@
         <v>154</v>
       </c>
       <c r="C45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>125</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>126</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>127</v>
       </c>
       <c r="B48" s="9"/>
       <c r="C48" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>128</v>
       </c>
       <c r="B49" s="9"/>
       <c r="C49" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>129</v>
       </c>
       <c r="B50" s="9"/>
       <c r="C50" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>130</v>
       </c>
       <c r="B51" s="9"/>
       <c r="C51" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>131</v>
       </c>
       <c r="B52" s="9"/>
       <c r="C52" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>132</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>133</v>
+        <v>307</v>
       </c>
       <c r="C54" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>134</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>155</v>
+        <v>308</v>
       </c>
       <c r="C56" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>136</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>137</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>138</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>139</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>140</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C61" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>141</v>
       </c>
       <c r="B62" s="6"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>142</v>
       </c>
       <c r="B63" s="6"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B65" s="6"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>144</v>
       </c>
       <c r="B66" s="6"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B67" s="6"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>146</v>
       </c>
       <c r="B68" s="6"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>147</v>
       </c>
       <c r="B69" s="6"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B70" s="6"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B71" s="6"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>149</v>
       </c>
       <c r="B72" s="6"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B73" s="6"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="6"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="6"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="6"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="6"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="6"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="6"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="6"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="6"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="6"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="6"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="6"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="6"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="6"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="6"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="6"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="6"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="6"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" s="6"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="6"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="6"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="6"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="6"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="6"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="6"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="6"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="6"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="6"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="6"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="6"/>
     </row>
   </sheetData>
@@ -2481,15 +2484,15 @@
       <selection activeCell="G122" sqref="G122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -2503,7 +2506,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
@@ -2517,258 +2520,258 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="D15" s="13"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="D17" s="13"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="D16" s="13"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>266</v>
-      </c>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="D22" s="13"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
+      <c r="D23" s="13"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="D24" s="13"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+      <c r="D25" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
+      <c r="D26" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
-        <v>273</v>
-      </c>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>83</v>
       </c>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>90</v>
       </c>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="D31" s="13"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="D32" s="13"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="D33" s="13"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
-        <v>278</v>
-      </c>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>97</v>
       </c>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="D36" s="13"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="D36" s="13"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
+      <c r="D37" s="13"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="D37" s="13"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
+      <c r="D38" s="13"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="D38" s="13"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
+      <c r="D39" s="13"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="D40" s="13"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="D39" s="13"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="D40" s="13"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
+      <c r="D41" s="13"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="D41" s="13"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
+      <c r="D42" s="13"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="D42" s="13"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
+      <c r="D43" s="13"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="D43" s="13"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="16" t="s">
-        <v>286</v>
-      </c>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>84</v>
       </c>
@@ -2776,7 +2779,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>85</v>
       </c>
@@ -2784,7 +2787,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>86</v>
       </c>
@@ -2792,7 +2795,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>88</v>
       </c>
@@ -2800,7 +2803,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>89</v>
       </c>
@@ -2808,7 +2811,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>91</v>
       </c>
@@ -2816,7 +2819,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>94</v>
       </c>
@@ -2824,7 +2827,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>96</v>
       </c>
@@ -2832,7 +2835,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>95</v>
       </c>
@@ -2840,7 +2843,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
         <v>92</v>
       </c>
@@ -2848,7 +2851,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>93</v>
       </c>
@@ -2856,7 +2859,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>36</v>
       </c>
@@ -2864,7 +2867,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
         <v>40</v>
       </c>
@@ -2872,7 +2875,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>39</v>
       </c>
@@ -2880,7 +2883,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
         <v>38</v>
       </c>
@@ -2888,7 +2891,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>34</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
         <v>37</v>
       </c>
@@ -2904,7 +2907,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>98</v>
       </c>
@@ -2912,7 +2915,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
         <v>99</v>
       </c>
@@ -2920,487 +2923,487 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="D64" s="13"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="D64" s="13"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="13" t="s">
+      <c r="D65" s="13"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D65" s="13"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="13" t="s">
+      <c r="D66" s="13"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D67" s="13"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="D66" s="13"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="13" t="s">
+      <c r="D68" s="13"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>290</v>
+      </c>
+      <c r="D69" s="13"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>222</v>
+      </c>
+      <c r="D70" s="13"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>291</v>
+      </c>
+      <c r="D71" s="13"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>292</v>
+      </c>
+      <c r="D72" s="13"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>250</v>
+      </c>
+      <c r="D73" s="13"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>215</v>
+      </c>
+      <c r="D74" s="13"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>293</v>
+      </c>
+      <c r="D75" s="13"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>294</v>
+      </c>
+      <c r="D76" s="13"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>203</v>
+      </c>
+      <c r="D77" s="13"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>295</v>
+      </c>
+      <c r="D78" s="13"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>296</v>
+      </c>
+      <c r="D79" s="13"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>297</v>
+      </c>
+      <c r="D80" s="13"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>298</v>
+      </c>
+      <c r="D81" s="13"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>299</v>
+      </c>
+      <c r="D82" s="13"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>300</v>
+      </c>
+      <c r="D83" s="13"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D84" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>247</v>
+      </c>
+      <c r="D85" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>249</v>
+      </c>
+      <c r="D86" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>218</v>
+      </c>
+      <c r="D87" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>301</v>
+      </c>
+      <c r="D88" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>209</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>230</v>
+      </c>
+      <c r="D90" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>212</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>242</v>
+      </c>
+      <c r="D92" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>227</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>243</v>
+      </c>
+      <c r="D94" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>244</v>
+      </c>
+      <c r="D95" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>302</v>
+      </c>
+      <c r="D96" s="13"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>303</v>
+      </c>
+      <c r="D97" s="13"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>304</v>
+      </c>
+      <c r="D98" s="13"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>305</v>
+      </c>
+      <c r="D99" s="13"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>306</v>
+      </c>
+      <c r="D100" s="13"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D101" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="D102" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D103" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="D104" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D105" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D106" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="D107" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D108" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="D109" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D110" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="D67" s="13"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="D68" s="13"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>291</v>
-      </c>
-      <c r="D69" s="13"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="D111" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="D112" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="D113" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D114" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="D115" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="D116" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D117" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="D118" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="D119" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D120" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="D121" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="D70" s="13"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>292</v>
-      </c>
-      <c r="D71" s="13"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>293</v>
-      </c>
-      <c r="D72" s="13"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>251</v>
-      </c>
-      <c r="D73" s="13"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>216</v>
-      </c>
-      <c r="D74" s="13"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>294</v>
-      </c>
-      <c r="D75" s="13"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>295</v>
-      </c>
-      <c r="D76" s="13"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="D122" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="D123" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="D124" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="D125" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D126" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="D127" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="D77" s="13"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>296</v>
-      </c>
-      <c r="D78" s="13"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>297</v>
-      </c>
-      <c r="D79" s="13"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>298</v>
-      </c>
-      <c r="D80" s="13"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>299</v>
-      </c>
-      <c r="D81" s="13"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>300</v>
-      </c>
-      <c r="D82" s="13"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>301</v>
-      </c>
-      <c r="D83" s="13"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>232</v>
-      </c>
-      <c r="D84" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>248</v>
-      </c>
-      <c r="D85" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>250</v>
-      </c>
-      <c r="D86" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>219</v>
-      </c>
-      <c r="D87" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>302</v>
-      </c>
-      <c r="D88" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>210</v>
-      </c>
-      <c r="D89" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>231</v>
-      </c>
-      <c r="D90" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>213</v>
-      </c>
-      <c r="D91" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>243</v>
-      </c>
-      <c r="D92" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>228</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>244</v>
-      </c>
-      <c r="D94" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>245</v>
-      </c>
-      <c r="D95" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>303</v>
-      </c>
-      <c r="D96" s="13"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>304</v>
-      </c>
-      <c r="D97" s="13"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>305</v>
-      </c>
-      <c r="D98" s="13"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>306</v>
-      </c>
-      <c r="D99" s="13"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>307</v>
-      </c>
-      <c r="D100" s="13"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="19" t="s">
-        <v>249</v>
-      </c>
-      <c r="D101" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="D102" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="D103" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="D104" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="D105" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="19" t="s">
+      <c r="D128" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="D106" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="D107" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="D108" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="D109" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="D110" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="19" t="s">
-        <v>240</v>
-      </c>
-      <c r="D111" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="D112" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="D113" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D114" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="19" t="s">
-        <v>234</v>
-      </c>
-      <c r="D115" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="19" t="s">
+      <c r="D129" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="19" t="s">
         <v>246</v>
-      </c>
-      <c r="D116" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="D117" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="D118" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="D119" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="D120" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="D121" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="D122" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="D123" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="D124" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="D125" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="D126" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="D127" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="D128" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="D129" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="19" t="s">
-        <v>247</v>
       </c>
       <c r="D130" t="s">
         <v>35</v>
@@ -3424,9 +3427,9 @@
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3437,7 +3440,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3445,7 +3448,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3453,7 +3456,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
fixed comm grps list and commodity list units
</commit_message>
<xml_diff>
--- a/config_data/mapping_v3.xlsx
+++ b/config_data/mapping_v3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8148"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="SEDOS_parameters" sheetId="5" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="307">
   <si>
     <t>TIMES</t>
   </si>
@@ -544,9 +544,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>FLO_EMISS</t>
   </si>
   <si>
     <t>1/NCAP_CHPR?</t>
@@ -1518,23 +1515,23 @@
   <dimension ref="A1:O120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1566,18 +1563,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1588,7 +1585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>81</v>
       </c>
@@ -1599,10 +1596,10 @@
         <v>82</v>
       </c>
       <c r="J4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>101</v>
       </c>
@@ -1610,7 +1607,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I5" t="s">
         <v>19</v>
@@ -1620,23 +1617,23 @@
       </c>
       <c r="N5" s="9"/>
       <c r="O5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N6" s="7"/>
       <c r="O6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1647,16 +1644,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>74</v>
       </c>
@@ -1664,10 +1661,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>103</v>
       </c>
@@ -1675,13 +1672,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>104</v>
       </c>
@@ -1689,13 +1686,13 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
@@ -1706,7 +1703,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>105</v>
       </c>
@@ -1714,13 +1711,13 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>106</v>
       </c>
@@ -1728,13 +1725,13 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>56</v>
       </c>
@@ -1745,7 +1742,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>107</v>
       </c>
@@ -1753,13 +1750,13 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>108</v>
       </c>
@@ -1767,13 +1764,13 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>109</v>
       </c>
@@ -1781,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
@@ -1792,13 +1789,13 @@
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -1812,7 +1809,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -1826,7 +1823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1837,7 +1834,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>110</v>
       </c>
@@ -1845,10 +1842,10 @@
         <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>111</v>
       </c>
@@ -1856,22 +1853,22 @@
         <v>150</v>
       </c>
       <c r="C24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J25" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -1882,7 +1879,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>66</v>
       </c>
@@ -1893,7 +1890,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>59</v>
       </c>
@@ -1904,7 +1901,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>113</v>
       </c>
@@ -1912,10 +1909,10 @@
         <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>78</v>
       </c>
@@ -1926,7 +1923,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>68</v>
       </c>
@@ -1937,7 +1934,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
@@ -1948,7 +1945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>114</v>
       </c>
@@ -1956,10 +1953,10 @@
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>70</v>
       </c>
@@ -1970,7 +1967,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>115</v>
       </c>
@@ -1978,7 +1975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>61</v>
       </c>
@@ -1989,7 +1986,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>116</v>
       </c>
@@ -2000,7 +1997,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>117</v>
       </c>
@@ -2014,7 +2011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>118</v>
       </c>
@@ -2028,7 +2025,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>119</v>
       </c>
@@ -2042,7 +2039,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -2050,129 +2047,127 @@
         <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>151</v>
-      </c>
+      <c r="B42" s="2"/>
       <c r="C42" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C44" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>125</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>126</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>127</v>
       </c>
       <c r="B48" s="9"/>
       <c r="C48" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>128</v>
       </c>
       <c r="B49" s="9"/>
       <c r="C49" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>129</v>
       </c>
       <c r="B50" s="9"/>
       <c r="C50" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>130</v>
       </c>
       <c r="B51" s="9"/>
       <c r="C51" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>131</v>
       </c>
       <c r="B52" s="9"/>
       <c r="C52" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>132</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>133</v>
       </c>
@@ -2180,290 +2175,290 @@
         <v>133</v>
       </c>
       <c r="C54" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>134</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C56" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>136</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>137</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>138</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>139</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>140</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C61" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>141</v>
       </c>
       <c r="B62" s="6"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>142</v>
       </c>
       <c r="B63" s="6"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B65" s="6"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>144</v>
       </c>
       <c r="B66" s="6"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B67" s="6"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>146</v>
       </c>
       <c r="B68" s="6"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>147</v>
       </c>
       <c r="B69" s="6"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B70" s="6"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B71" s="6"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>149</v>
       </c>
       <c r="B72" s="6"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B73" s="6"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="6"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="6"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="6"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="6"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="6"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="6"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="6"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="6"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="6"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="6"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="6"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="6"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="6"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="6"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="6"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="6"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="6"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" s="6"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="6"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="6"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="6"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="6"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="6"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="6"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="6"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="6"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="6"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="6"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="6"/>
     </row>
   </sheetData>
@@ -2481,15 +2476,15 @@
       <selection activeCell="G122" sqref="G122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -2503,7 +2498,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
@@ -2517,258 +2512,258 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="D15" s="13"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="D17" s="13"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="D16" s="13"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>266</v>
-      </c>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="D22" s="13"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
+      <c r="D23" s="13"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="D24" s="13"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+      <c r="D25" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
+      <c r="D26" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
-        <v>273</v>
-      </c>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>83</v>
       </c>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>90</v>
       </c>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="D31" s="13"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="D32" s="13"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="D33" s="13"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
-        <v>278</v>
-      </c>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>97</v>
       </c>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="D36" s="13"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="D36" s="13"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
+      <c r="D37" s="13"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="D37" s="13"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
+      <c r="D38" s="13"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="D38" s="13"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
+      <c r="D39" s="13"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="D40" s="13"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="D39" s="13"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="D40" s="13"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
+      <c r="D41" s="13"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="D41" s="13"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
+      <c r="D42" s="13"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="D42" s="13"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
+      <c r="D43" s="13"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="D43" s="13"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="16" t="s">
-        <v>286</v>
-      </c>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>84</v>
       </c>
@@ -2776,7 +2771,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>85</v>
       </c>
@@ -2784,7 +2779,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>86</v>
       </c>
@@ -2792,7 +2787,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>88</v>
       </c>
@@ -2800,7 +2795,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>89</v>
       </c>
@@ -2808,7 +2803,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>91</v>
       </c>
@@ -2816,7 +2811,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>94</v>
       </c>
@@ -2824,7 +2819,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>96</v>
       </c>
@@ -2832,7 +2827,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>95</v>
       </c>
@@ -2840,7 +2835,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
         <v>92</v>
       </c>
@@ -2848,7 +2843,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>93</v>
       </c>
@@ -2856,7 +2851,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>36</v>
       </c>
@@ -2864,7 +2859,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
         <v>40</v>
       </c>
@@ -2872,7 +2867,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>39</v>
       </c>
@@ -2880,7 +2875,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
         <v>38</v>
       </c>
@@ -2888,7 +2883,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>34</v>
       </c>
@@ -2896,7 +2891,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
         <v>37</v>
       </c>
@@ -2904,7 +2899,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>98</v>
       </c>
@@ -2912,7 +2907,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
         <v>99</v>
       </c>
@@ -2920,487 +2915,487 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="D64" s="13"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="D64" s="13"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="13" t="s">
+      <c r="D65" s="13"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D65" s="13"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="13" t="s">
+      <c r="D66" s="13"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D67" s="13"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="D66" s="13"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="13" t="s">
+      <c r="D68" s="13"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>290</v>
+      </c>
+      <c r="D69" s="13"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>222</v>
+      </c>
+      <c r="D70" s="13"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>291</v>
+      </c>
+      <c r="D71" s="13"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>292</v>
+      </c>
+      <c r="D72" s="13"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>250</v>
+      </c>
+      <c r="D73" s="13"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>215</v>
+      </c>
+      <c r="D74" s="13"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>293</v>
+      </c>
+      <c r="D75" s="13"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>294</v>
+      </c>
+      <c r="D76" s="13"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>203</v>
+      </c>
+      <c r="D77" s="13"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>295</v>
+      </c>
+      <c r="D78" s="13"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>296</v>
+      </c>
+      <c r="D79" s="13"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>297</v>
+      </c>
+      <c r="D80" s="13"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>298</v>
+      </c>
+      <c r="D81" s="13"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>299</v>
+      </c>
+      <c r="D82" s="13"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>300</v>
+      </c>
+      <c r="D83" s="13"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D84" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>247</v>
+      </c>
+      <c r="D85" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>249</v>
+      </c>
+      <c r="D86" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>218</v>
+      </c>
+      <c r="D87" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>301</v>
+      </c>
+      <c r="D88" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>209</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>230</v>
+      </c>
+      <c r="D90" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>212</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>242</v>
+      </c>
+      <c r="D92" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>227</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>243</v>
+      </c>
+      <c r="D94" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>244</v>
+      </c>
+      <c r="D95" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>302</v>
+      </c>
+      <c r="D96" s="13"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>303</v>
+      </c>
+      <c r="D97" s="13"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>304</v>
+      </c>
+      <c r="D98" s="13"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>305</v>
+      </c>
+      <c r="D99" s="13"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>306</v>
+      </c>
+      <c r="D100" s="13"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D101" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="D102" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D103" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="D104" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D105" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D106" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="D107" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D108" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="D109" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D110" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="D67" s="13"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="D68" s="13"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>291</v>
-      </c>
-      <c r="D69" s="13"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="D111" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="D112" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="D113" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D114" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="D115" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="D116" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D117" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="D118" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="D119" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D120" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="D121" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="D70" s="13"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>292</v>
-      </c>
-      <c r="D71" s="13"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>293</v>
-      </c>
-      <c r="D72" s="13"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>251</v>
-      </c>
-      <c r="D73" s="13"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>216</v>
-      </c>
-      <c r="D74" s="13"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>294</v>
-      </c>
-      <c r="D75" s="13"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>295</v>
-      </c>
-      <c r="D76" s="13"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="D122" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="D123" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="D124" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="D125" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D126" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="D127" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="D77" s="13"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>296</v>
-      </c>
-      <c r="D78" s="13"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>297</v>
-      </c>
-      <c r="D79" s="13"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>298</v>
-      </c>
-      <c r="D80" s="13"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>299</v>
-      </c>
-      <c r="D81" s="13"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>300</v>
-      </c>
-      <c r="D82" s="13"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>301</v>
-      </c>
-      <c r="D83" s="13"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>232</v>
-      </c>
-      <c r="D84" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>248</v>
-      </c>
-      <c r="D85" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>250</v>
-      </c>
-      <c r="D86" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>219</v>
-      </c>
-      <c r="D87" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>302</v>
-      </c>
-      <c r="D88" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>210</v>
-      </c>
-      <c r="D89" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>231</v>
-      </c>
-      <c r="D90" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>213</v>
-      </c>
-      <c r="D91" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>243</v>
-      </c>
-      <c r="D92" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>228</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>244</v>
-      </c>
-      <c r="D94" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>245</v>
-      </c>
-      <c r="D95" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>303</v>
-      </c>
-      <c r="D96" s="13"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>304</v>
-      </c>
-      <c r="D97" s="13"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>305</v>
-      </c>
-      <c r="D98" s="13"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>306</v>
-      </c>
-      <c r="D99" s="13"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>307</v>
-      </c>
-      <c r="D100" s="13"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="19" t="s">
-        <v>249</v>
-      </c>
-      <c r="D101" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="D102" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="D103" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="D104" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="D105" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="19" t="s">
+      <c r="D128" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="D106" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="D107" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="D108" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="D109" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="D110" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="19" t="s">
-        <v>240</v>
-      </c>
-      <c r="D111" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="D112" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="D113" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D114" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="19" t="s">
-        <v>234</v>
-      </c>
-      <c r="D115" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="19" t="s">
+      <c r="D129" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="19" t="s">
         <v>246</v>
-      </c>
-      <c r="D116" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="D117" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="D118" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="D119" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="D120" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="D121" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="D122" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="D123" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="D124" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="D125" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="D126" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="D127" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="D128" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="D129" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="19" t="s">
-        <v>247</v>
       </c>
       <c r="D130" t="s">
         <v>35</v>
@@ -3424,9 +3419,9 @@
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3437,7 +3432,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3445,7 +3440,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3453,7 +3448,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
updated mapping and input
</commit_message>
<xml_diff>
--- a/config_data/mapping_v3.xlsx
+++ b/config_data/mapping_v3.xlsx
@@ -15,6 +15,7 @@
     <sheet name="SEDOS_parameters" sheetId="5" r:id="rId1"/>
     <sheet name="commodity_set" sheetId="4" r:id="rId2"/>
     <sheet name="limits" sheetId="3" r:id="rId3"/>
+    <sheet name="units" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">commodity_set!$A$1:$A$130</definedName>
@@ -91,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="327">
   <si>
     <t>TIMES</t>
   </si>
@@ -1012,6 +1013,66 @@
   </si>
   <si>
     <t>exo_agri_livestock</t>
+  </si>
+  <si>
+    <t>conversion_factor</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>Kt</t>
+  </si>
+  <si>
+    <t>PJ</t>
+  </si>
+  <si>
+    <t>Million units</t>
+  </si>
+  <si>
+    <t>Mt</t>
+  </si>
+  <si>
+    <t>M€</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>vehicle</t>
+  </si>
+  <si>
+    <t>KW</t>
+  </si>
+  <si>
+    <t>KWh</t>
+  </si>
+  <si>
+    <t>pkm</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>persons</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>tkm</t>
+  </si>
+  <si>
+    <t>vehicles</t>
+  </si>
+  <si>
+    <t>100km</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1186,6 +1247,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal 10" xfId="1"/>
@@ -1515,7 +1578,7 @@
   <dimension ref="A1:O120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3459,4 +3522,254 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="C10" s="13">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="C12" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="C13" s="21">
+        <v>3.6E-9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="C14" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="C16" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="C17" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="C18" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="C19" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="C20" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="C21" s="13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>